<commit_message>
Actualización en referencia única pro estudio y visualización de errores. Se borra de la DB al eliminarse.
</commit_message>
<xml_diff>
--- a/bateria_tests/estudios/plantilla_estudios_bueno.xlsx
+++ b/bateria_tests/estudios/plantilla_estudios_bueno.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\OneDrive\Documentos\Practicas_UOC\datos_muestras\bateria_tests\estudios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0627F2-4AEF-4C74-B55A-5CCC5A550B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54095606-1B93-43E3-A753-EAE02FA69B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="1060" windowWidth="20570" windowHeight="7450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Descripción</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>ELA</t>
-  </si>
-  <si>
-    <t>Papa</t>
   </si>
 </sst>
 </file>
@@ -402,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -518,26 +515,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización fechas inicio y término - Verificar formato y luego que inico antes o igual que término. Al subir manualmente un estudio o editarlo, verifica nombre y referencia
</commit_message>
<xml_diff>
--- a/bateria_tests/estudios/plantilla_estudios_bueno.xlsx
+++ b/bateria_tests/estudios/plantilla_estudios_bueno.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\OneDrive\Documentos\Practicas_UOC\datos_muestras\bateria_tests\estudios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54095606-1B93-43E3-A753-EAE02FA69B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594A5150-0844-449D-AEEB-269068332746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="1060" windowWidth="20570" windowHeight="7450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,10 +115,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,7 +403,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="A6:F6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,11 +446,11 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
+      <c r="D2" s="3">
+        <v>38772</v>
+      </c>
+      <c r="E2" s="3">
+        <v>45716</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -465,11 +466,11 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
+      <c r="D3" s="3">
+        <v>38773</v>
+      </c>
+      <c r="E3" s="3">
+        <v>46021</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -485,11 +486,11 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
+      <c r="D4" s="3">
+        <v>38774</v>
+      </c>
+      <c r="E4" s="3">
+        <v>46368</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -505,11 +506,11 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
+      <c r="D5" s="3">
+        <v>38775</v>
+      </c>
+      <c r="E5" s="3">
+        <v>47832</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>

</xml_diff>